<commit_message>
input on excel works - python scripts work
</commit_message>
<xml_diff>
--- a/Building folder/Schade kosten Kastanjelaan 232, Bergen op Zoom.xlsx
+++ b/Building folder/Schade kosten Kastanjelaan 232, Bergen op Zoom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ryanrent.sharepoint.com/sites/RyanRent/Gedeelde documenten/General/01_RyanRent&amp;Co/Aljereau/Eindafrekening Generator/Building folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE745D62-12FC-B641-8E20-A6E62E9A448F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{FE745D62-12FC-B641-8E20-A6E62E9A448F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F909A44-C36E-C04D-9F19-7DF3C64D7F1A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" activeTab="1" xr2:uid="{EFE5ECCD-C285-405F-B177-44F960C98771}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Kosten</t>
   </si>
@@ -66,15 +66,9 @@
     <t>Schoonmaak + afvoeren afval</t>
   </si>
   <si>
-    <t>Bij</t>
-  </si>
-  <si>
     <t>Uren</t>
   </si>
   <si>
-    <t>Tarief</t>
-  </si>
-  <si>
     <t>Extra Kosten</t>
   </si>
   <si>
@@ -87,7 +81,7 @@
     <t>EXTRA</t>
   </si>
   <si>
-    <t>EINSCHOONMAAK AANBETALING</t>
+    <t>Tarief per uur</t>
   </si>
 </sst>
 </file>
@@ -149,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -159,6 +153,9 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +609,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3792F968-B54D-4749-A570-59C1EECA7990}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A10" sqref="A10:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -625,31 +622,33 @@
     <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3">
         <v>100</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="7">
+        <v>10</v>
+      </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -661,7 +660,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -672,11 +671,8 @@
       <c r="D4" s="4">
         <v>97.5</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -687,39 +683,39 @@
         <v>46.4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5">
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>500</v>
@@ -730,9 +726,9 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -743,9 +739,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B12" s="3">
         <v>60</v>
@@ -756,18 +752,18 @@
         <v>208.6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="5">
         <f>SUM(D10:D12)</f>
         <v>868.6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -778,14 +774,11 @@
         <v>2756.1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D16" s="1"/>
-      <c r="G16" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" s="1"/>
@@ -1115,16 +1108,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2C9E4-7EFA-4A86-B783-366B17446975}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7c6541c9-858d-46cc-aee4-1fa681dc1bd6"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7c6541c9-858d-46cc-aee4-1fa681dc1bd6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>